<commit_message>
Agrego TS, BO y FF a secuencia
</commit_message>
<xml_diff>
--- a/src/competencia3/secuencia.xlsx
+++ b/src/competencia3/secuencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\competencia3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E676A6-2405-4D2C-A072-583536B0A789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28929CB9-9051-471E-BE09-5A6A153157B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
+    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>SCRIPT</t>
   </si>
@@ -126,6 +126,32 @@
   </si>
   <si>
     <t>Se colgó con 256 gigas de ram</t>
+  </si>
+  <si>
+    <t>Todos los campos del paso anterior</t>
+  </si>
+  <si>
+    <t>Training strategy. Separar datasets: bo, train y test</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>Dataset del paso anterior</t>
+  </si>
+  <si>
+    <t>941_HT</t>
+  </si>
+  <si>
+    <t>exp/TS9310/dataset_future.csv.gz #futuro
+exp/TS9310/dataset_train_final.csv.gz #para entrenar modelo final
+exp/TS9310/dataset_training.csv.gz #para hacer bo</t>
+  </si>
+  <si>
+    <t>exp/TS9310/dataset_training.csv.gz</t>
+  </si>
+  <si>
+    <t>exp/HT9410/dataset_training.csv.gz</t>
   </si>
 </sst>
 </file>
@@ -161,8 +187,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,19 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A84B28-8535-45EF-B1C2-8C54628A6A9E}">
-  <dimension ref="A3:G8"/>
+  <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.140625" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -621,6 +650,40 @@
         <v>28</v>
       </c>
     </row>
+    <row r="9" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>931</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agrego comentarios y nuevos pasos
</commit_message>
<xml_diff>
--- a/src/competencia3/secuencia.xlsx
+++ b/src/competencia3/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\competencia3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28929CB9-9051-471E-BE09-5A6A153157B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04794B06-EAB3-49B0-B49B-581A38134DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>SCRIPT</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>OBSERVACIONES</t>
-  </si>
-  <si>
-    <t>Consumió 500 gigas de ram</t>
   </si>
   <si>
     <t>Se colgó con 256 gigas de ram</t>
@@ -152,6 +149,15 @@
   </si>
   <si>
     <t>exp/HT9410/dataset_training.csv.gz</t>
+  </si>
+  <si>
+    <t>Consumió 500 gigas de ram. Dejó 1896 vbles</t>
+  </si>
+  <si>
+    <t>Modelo final</t>
+  </si>
+  <si>
+    <t>23 horas</t>
   </si>
 </sst>
 </file>
@@ -506,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A84B28-8535-45EF-B1C2-8C54628A6A9E}">
-  <dimension ref="A3:G10"/>
+  <dimension ref="A3:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +630,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -647,15 +653,18 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>931</v>
@@ -664,24 +673,35 @@
         <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
-        <v>37</v>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego modelo final con corte en 15.000
</commit_message>
<xml_diff>
--- a/src/competencia3/secuencia.xlsx
+++ b/src/competencia3/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\competencia3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04794B06-EAB3-49B0-B49B-581A38134DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DB9AB1-1C81-449A-91CB-7579B7D98625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>SCRIPT</t>
   </si>
@@ -158,6 +158,24 @@
   </si>
   <si>
     <t>23 horas</t>
+  </si>
+  <si>
+    <t>exp/ZZ9410</t>
+  </si>
+  <si>
+    <t>Entrenar el modelo final</t>
+  </si>
+  <si>
+    <t>991_ZZ_lightgbm_15000</t>
+  </si>
+  <si>
+    <t>991_ZZ_lightgbm</t>
+  </si>
+  <si>
+    <t>Entrenar el modelo final. Cortes hasta 15000</t>
+  </si>
+  <si>
+    <t>exp/ZZ9411</t>
   </si>
 </sst>
 </file>
@@ -512,17 +530,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A84B28-8535-45EF-B1C2-8C54628A6A9E}">
-  <dimension ref="A3:G11"/>
+  <dimension ref="A3:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60" customWidth="1"/>
   </cols>
@@ -700,8 +718,40 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
       <c r="B11" t="s">
         <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego entrenamiento de 9 meses
</commit_message>
<xml_diff>
--- a/src/competencia3/secuencia.xlsx
+++ b/src/competencia3/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\competencia3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DB9AB1-1C81-449A-91CB-7579B7D98625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E081631-5EEB-474B-9BCE-FE5B5C6BC68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>SCRIPT</t>
   </si>
@@ -176,6 +176,17 @@
   </si>
   <si>
     <t>exp/ZZ9411</t>
+  </si>
+  <si>
+    <t>exp/TS9311/dataset_future.csv.gz #futuro
+exp/TS9311/dataset_train_final.csv.gz #para entrenar modelo final
+exp/TS9311/dataset_training.csv.gz #para hacer bo</t>
+  </si>
+  <si>
+    <t>EXPERMENTO CON 3 MESES DE TRAINING</t>
+  </si>
+  <si>
+    <t>EXPERMENTO CON 9 MESES DE TRAINING</t>
   </si>
 </sst>
 </file>
@@ -530,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A84B28-8535-45EF-B1C2-8C54628A6A9E}">
-  <dimension ref="A3:G12"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,83 +685,164 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9">
-        <v>931</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>931</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E14" t="s">
         <v>36</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>9312</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agrego HT, final model y secuencia con entrenamiento de 9 meses
</commit_message>
<xml_diff>
--- a/src/competencia3/secuencia.xlsx
+++ b/src/competencia3/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\competencia3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E081631-5EEB-474B-9BCE-FE5B5C6BC68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81B209F-7B90-4EC5-B8C6-A911CB4DF3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>SCRIPT</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>EXPERMENTO CON 9 MESES DE TRAINING</t>
+  </si>
+  <si>
+    <t>exp/TS9311/dataset_training.csv.gz</t>
+  </si>
+  <si>
+    <t>exp/HT9411/dataset_training.csv.gz</t>
+  </si>
+  <si>
+    <t>exp/ZZ9412</t>
   </si>
 </sst>
 </file>
@@ -544,7 +553,7 @@
   <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,10 +815,10 @@
         <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -823,10 +832,10 @@
         <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,10 +849,10 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego experimento con 9 meses
</commit_message>
<xml_diff>
--- a/src/competencia3/secuencia.xlsx
+++ b/src/competencia3/secuencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\competencia3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81B209F-7B90-4EC5-B8C6-A911CB4DF3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF397FBE-189F-4123-837E-C2845A92F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9679DE49-D82E-4F7E-A9E2-7A6BA30DF2EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>SCRIPT</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>exp/ZZ9412</t>
+  </si>
+  <si>
+    <t>942_HT</t>
+  </si>
+  <si>
+    <t>992_ZZ_lightgbm_15000</t>
+  </si>
+  <si>
+    <t>3 días</t>
   </si>
 </sst>
 </file>
@@ -550,16 +559,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A84B28-8535-45EF-B1C2-8C54628A6A9E}">
-  <dimension ref="A3:G22"/>
+  <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60" customWidth="1"/>
@@ -782,12 +791,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -804,7 +816,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -812,7 +827,7 @@
         <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>49</v>
@@ -820,38 +835,27 @@
       <c r="F20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
         <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>